<commit_message>
adding type of link test 1
</commit_message>
<xml_diff>
--- a/regulondb/collection/link/sRNA_Gene.xlsx
+++ b/regulondb/collection/link/sRNA_Gene.xlsx
@@ -830,9 +830,6 @@
     <t>DNA strand of the regulated gene</t>
   </si>
   <si>
-    <t>Function (+ activation, - repression, +- dual, ? unknown)</t>
-  </si>
-  <si>
     <t>Regulation type</t>
   </si>
   <si>
@@ -1038,6 +1035,10 @@
   </si>
   <si>
     <t>RdlC</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Function</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1980,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A228" sqref="A228"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
@@ -1991,7 +1992,7 @@
     <col min="3" max="3" width="45" customWidth="1"/>
     <col min="4" max="4" width="47.125" customWidth="1"/>
     <col min="5" max="5" width="34" customWidth="1"/>
-    <col min="6" max="6" width="58.5" customWidth="1"/>
+    <col min="6" max="6" width="9.875" customWidth="1"/>
     <col min="7" max="7" width="67.875" customWidth="1"/>
     <col min="8" max="8" width="20.5" customWidth="1"/>
     <col min="9" max="9" width="35.5" customWidth="1"/>
@@ -2000,10 +2001,10 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" t="s">
         <v>274</v>
-      </c>
-      <c r="B1" t="s">
-        <v>275</v>
       </c>
       <c r="C1" t="s">
         <v>266</v>
@@ -2015,24 +2016,24 @@
         <v>268</v>
       </c>
       <c r="F1" t="s">
+        <v>322</v>
+      </c>
+      <c r="G1" t="s">
+        <v>270</v>
+      </c>
+      <c r="H1" t="s">
         <v>269</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>271</v>
       </c>
-      <c r="H1" t="s">
-        <v>270</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>272</v>
-      </c>
-      <c r="J1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -2055,7 +2056,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -2118,7 +2119,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -2150,7 +2151,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -2182,7 +2183,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -2214,7 +2215,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
@@ -2237,7 +2238,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
@@ -2260,7 +2261,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
@@ -2283,7 +2284,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -2306,7 +2307,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
@@ -2329,7 +2330,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
@@ -2352,7 +2353,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
@@ -2375,7 +2376,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
@@ -2398,7 +2399,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
@@ -2421,7 +2422,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B18" t="s">
         <v>31</v>
@@ -2444,7 +2445,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B19" t="s">
         <v>32</v>
@@ -2467,7 +2468,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B20" t="s">
         <v>33</v>
@@ -2490,7 +2491,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B21" t="s">
         <v>34</v>
@@ -2504,7 +2505,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B22" t="s">
         <v>35</v>
@@ -2527,7 +2528,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
@@ -2550,7 +2551,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B24" t="s">
         <v>37</v>
@@ -2573,7 +2574,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B25" t="s">
         <v>38</v>
@@ -2593,7 +2594,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B26" t="s">
         <v>39</v>
@@ -2616,7 +2617,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B27" t="s">
         <v>40</v>
@@ -2648,7 +2649,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B28" t="s">
         <v>42</v>
@@ -2677,7 +2678,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B29" t="s">
         <v>44</v>
@@ -2700,7 +2701,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B30" t="s">
         <v>45</v>
@@ -2732,7 +2733,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B31" t="s">
         <v>47</v>
@@ -2755,7 +2756,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B32" t="s">
         <v>48</v>
@@ -2778,7 +2779,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B33" t="s">
         <v>49</v>
@@ -2801,7 +2802,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B34" t="s">
         <v>50</v>
@@ -2824,7 +2825,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B35" t="s">
         <v>51</v>
@@ -2853,7 +2854,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
@@ -2867,7 +2868,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B37" t="s">
         <v>53</v>
@@ -2878,7 +2879,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B38" t="s">
         <v>54</v>
@@ -2892,7 +2893,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -2984,7 +2985,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B43" t="s">
         <v>59</v>
@@ -3007,7 +3008,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B44" t="s">
         <v>60</v>
@@ -3027,7 +3028,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B45" t="s">
         <v>62</v>
@@ -3059,7 +3060,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B46" t="s">
         <v>66</v>
@@ -3079,7 +3080,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B47" t="s">
         <v>67</v>
@@ -3111,7 +3112,7 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B48" t="s">
         <v>69</v>
@@ -3140,7 +3141,7 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B49" t="s">
         <v>71</v>
@@ -3163,7 +3164,7 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B50" t="s">
         <v>74</v>
@@ -3186,7 +3187,7 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B51" t="s">
         <v>75</v>
@@ -3209,7 +3210,7 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B52" t="s">
         <v>76</v>
@@ -3241,7 +3242,7 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B53" t="s">
         <v>79</v>
@@ -3273,7 +3274,7 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B54" t="s">
         <v>81</v>
@@ -3296,7 +3297,7 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B55" t="s">
         <v>82</v>
@@ -3319,7 +3320,7 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B56" t="s">
         <v>83</v>
@@ -3342,7 +3343,7 @@
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B57" t="s">
         <v>84</v>
@@ -3362,7 +3363,7 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B58" t="s">
         <v>85</v>
@@ -3385,7 +3386,7 @@
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B59" t="s">
         <v>86</v>
@@ -3408,7 +3409,7 @@
     </row>
     <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B60" t="s">
         <v>87</v>
@@ -3431,7 +3432,7 @@
     </row>
     <row r="61" spans="1:10">
       <c r="A61" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B61" t="s">
         <v>88</v>
@@ -3454,7 +3455,7 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B62" t="s">
         <v>89</v>
@@ -3477,7 +3478,7 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B63" t="s">
         <v>90</v>
@@ -3500,7 +3501,7 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B64" t="s">
         <v>91</v>
@@ -3523,7 +3524,7 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B65" t="s">
         <v>92</v>
@@ -3546,7 +3547,7 @@
     </row>
     <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B66" t="s">
         <v>93</v>
@@ -3575,7 +3576,7 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B67" t="s">
         <v>93</v>
@@ -3604,7 +3605,7 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B68" t="s">
         <v>96</v>
@@ -3633,7 +3634,7 @@
     </row>
     <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B69" t="s">
         <v>98</v>
@@ -3662,7 +3663,7 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B70" t="s">
         <v>6</v>
@@ -3694,7 +3695,7 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B71" t="s">
         <v>101</v>
@@ -3726,7 +3727,7 @@
     </row>
     <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B72" t="s">
         <v>104</v>
@@ -3746,7 +3747,7 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B73" t="s">
         <v>105</v>
@@ -3766,7 +3767,7 @@
     </row>
     <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B74" t="s">
         <v>106</v>
@@ -3786,7 +3787,7 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B75" t="s">
         <v>107</v>
@@ -3806,7 +3807,7 @@
     </row>
     <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B76" t="s">
         <v>108</v>
@@ -3838,7 +3839,7 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B77" t="s">
         <v>110</v>
@@ -3870,7 +3871,7 @@
     </row>
     <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B78" t="s">
         <v>112</v>
@@ -3902,7 +3903,7 @@
     </row>
     <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B79" t="s">
         <v>114</v>
@@ -3922,7 +3923,7 @@
     </row>
     <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B80" t="s">
         <v>115</v>
@@ -3942,7 +3943,7 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B81" t="s">
         <v>0</v>
@@ -4003,7 +4004,7 @@
     </row>
     <row r="83" spans="1:10">
       <c r="A83" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B83" t="s">
         <v>121</v>
@@ -4035,7 +4036,7 @@
     </row>
     <row r="84" spans="1:10">
       <c r="A84" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B84" t="s">
         <v>123</v>
@@ -4067,7 +4068,7 @@
     </row>
     <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B85" t="s">
         <v>125</v>
@@ -4081,7 +4082,7 @@
     </row>
     <row r="86" spans="1:10">
       <c r="A86" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B86" t="s">
         <v>126</v>
@@ -4113,7 +4114,7 @@
     </row>
     <row r="87" spans="1:10">
       <c r="A87" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B87" t="s">
         <v>128</v>
@@ -4133,7 +4134,7 @@
     </row>
     <row r="88" spans="1:10">
       <c r="A88" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B88" t="s">
         <v>129</v>
@@ -4156,7 +4157,7 @@
     </row>
     <row r="89" spans="1:10">
       <c r="A89" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B89" t="s">
         <v>130</v>
@@ -4179,7 +4180,7 @@
     </row>
     <row r="90" spans="1:10">
       <c r="A90" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B90" t="s">
         <v>133</v>
@@ -4199,7 +4200,7 @@
     </row>
     <row r="91" spans="1:10">
       <c r="A91" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B91" t="s">
         <v>84</v>
@@ -4228,7 +4229,7 @@
     </row>
     <row r="92" spans="1:10">
       <c r="A92" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B92" t="s">
         <v>33</v>
@@ -4260,7 +4261,7 @@
     </row>
     <row r="93" spans="1:10">
       <c r="A93" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B93" t="s">
         <v>101</v>
@@ -4292,7 +4293,7 @@
     </row>
     <row r="94" spans="1:10">
       <c r="A94" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B94" t="s">
         <v>139</v>
@@ -4315,7 +4316,7 @@
     </row>
     <row r="95" spans="1:10">
       <c r="A95" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B95" t="s">
         <v>140</v>
@@ -4338,7 +4339,7 @@
     </row>
     <row r="96" spans="1:10">
       <c r="A96" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B96" t="s">
         <v>141</v>
@@ -4361,7 +4362,7 @@
     </row>
     <row r="97" spans="1:10">
       <c r="A97" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B97" t="s">
         <v>142</v>
@@ -4384,7 +4385,7 @@
     </row>
     <row r="98" spans="1:10">
       <c r="A98" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B98" t="s">
         <v>143</v>
@@ -4407,7 +4408,7 @@
     </row>
     <row r="99" spans="1:10">
       <c r="A99" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B99" t="s">
         <v>144</v>
@@ -4430,7 +4431,7 @@
     </row>
     <row r="100" spans="1:10">
       <c r="A100" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B100" t="s">
         <v>145</v>
@@ -4453,7 +4454,7 @@
     </row>
     <row r="101" spans="1:10">
       <c r="A101" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B101" t="s">
         <v>146</v>
@@ -4485,7 +4486,7 @@
     </row>
     <row r="102" spans="1:10">
       <c r="A102" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B102" t="s">
         <v>149</v>
@@ -4508,7 +4509,7 @@
     </row>
     <row r="103" spans="1:10">
       <c r="A103" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B103" t="s">
         <v>150</v>
@@ -4531,7 +4532,7 @@
     </row>
     <row r="104" spans="1:10">
       <c r="A104" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B104" t="s">
         <v>151</v>
@@ -4554,7 +4555,7 @@
     </row>
     <row r="105" spans="1:10">
       <c r="A105" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B105" t="s">
         <v>152</v>
@@ -4577,7 +4578,7 @@
     </row>
     <row r="106" spans="1:10">
       <c r="A106" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B106" t="s">
         <v>153</v>
@@ -4600,7 +4601,7 @@
     </row>
     <row r="107" spans="1:10">
       <c r="A107" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B107" t="s">
         <v>154</v>
@@ -4623,7 +4624,7 @@
     </row>
     <row r="108" spans="1:10">
       <c r="A108" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B108" t="s">
         <v>154</v>
@@ -4646,7 +4647,7 @@
     </row>
     <row r="109" spans="1:10">
       <c r="A109" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B109" t="s">
         <v>155</v>
@@ -4669,7 +4670,7 @@
     </row>
     <row r="110" spans="1:10">
       <c r="A110" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B110" t="s">
         <v>156</v>
@@ -4692,7 +4693,7 @@
     </row>
     <row r="111" spans="1:10">
       <c r="A111" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B111" t="s">
         <v>157</v>
@@ -4724,7 +4725,7 @@
     </row>
     <row r="112" spans="1:10">
       <c r="A112" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B112" t="s">
         <v>159</v>
@@ -4756,7 +4757,7 @@
     </row>
     <row r="113" spans="1:10">
       <c r="A113" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B113" t="s">
         <v>161</v>
@@ -4779,7 +4780,7 @@
     </row>
     <row r="114" spans="1:10">
       <c r="A114" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B114" t="s">
         <v>162</v>
@@ -4802,7 +4803,7 @@
     </row>
     <row r="115" spans="1:10">
       <c r="A115" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B115" t="s">
         <v>163</v>
@@ -4825,7 +4826,7 @@
     </row>
     <row r="116" spans="1:10">
       <c r="A116" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B116" t="s">
         <v>164</v>
@@ -4848,7 +4849,7 @@
     </row>
     <row r="117" spans="1:10">
       <c r="A117" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B117" t="s">
         <v>165</v>
@@ -4871,7 +4872,7 @@
     </row>
     <row r="118" spans="1:10">
       <c r="A118" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B118" t="s">
         <v>166</v>
@@ -4894,7 +4895,7 @@
     </row>
     <row r="119" spans="1:10">
       <c r="A119" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B119" t="s">
         <v>167</v>
@@ -4917,7 +4918,7 @@
     </row>
     <row r="120" spans="1:10">
       <c r="A120" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B120" t="s">
         <v>168</v>
@@ -4940,7 +4941,7 @@
     </row>
     <row r="121" spans="1:10">
       <c r="A121" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B121" t="s">
         <v>169</v>
@@ -4963,7 +4964,7 @@
     </row>
     <row r="122" spans="1:10">
       <c r="A122" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B122" t="s">
         <v>170</v>
@@ -4986,7 +4987,7 @@
     </row>
     <row r="123" spans="1:10">
       <c r="A123" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B123" t="s">
         <v>171</v>
@@ -5009,7 +5010,7 @@
     </row>
     <row r="124" spans="1:10">
       <c r="A124" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B124" t="s">
         <v>172</v>
@@ -5032,7 +5033,7 @@
     </row>
     <row r="125" spans="1:10">
       <c r="A125" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B125" t="s">
         <v>173</v>
@@ -5055,7 +5056,7 @@
     </row>
     <row r="126" spans="1:10">
       <c r="A126" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B126" t="s">
         <v>174</v>
@@ -5078,7 +5079,7 @@
     </row>
     <row r="127" spans="1:10">
       <c r="A127" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B127" t="s">
         <v>175</v>
@@ -5101,7 +5102,7 @@
     </row>
     <row r="128" spans="1:10">
       <c r="A128" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B128" t="s">
         <v>176</v>
@@ -5124,7 +5125,7 @@
     </row>
     <row r="129" spans="1:10">
       <c r="A129" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B129" t="s">
         <v>177</v>
@@ -5147,7 +5148,7 @@
     </row>
     <row r="130" spans="1:10">
       <c r="A130" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B130" t="s">
         <v>178</v>
@@ -5170,7 +5171,7 @@
     </row>
     <row r="131" spans="1:10">
       <c r="A131" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B131" t="s">
         <v>179</v>
@@ -5193,7 +5194,7 @@
     </row>
     <row r="132" spans="1:10">
       <c r="A132" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B132" t="s">
         <v>180</v>
@@ -5225,7 +5226,7 @@
     </row>
     <row r="133" spans="1:10">
       <c r="A133" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B133" t="s">
         <v>182</v>
@@ -5257,7 +5258,7 @@
     </row>
     <row r="134" spans="1:10">
       <c r="A134" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B134" t="s">
         <v>184</v>
@@ -5280,7 +5281,7 @@
     </row>
     <row r="135" spans="1:10">
       <c r="A135" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B135" t="s">
         <v>185</v>
@@ -5303,7 +5304,7 @@
     </row>
     <row r="136" spans="1:10">
       <c r="A136" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B136" t="s">
         <v>186</v>
@@ -5326,7 +5327,7 @@
     </row>
     <row r="137" spans="1:10">
       <c r="A137" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B137" t="s">
         <v>187</v>
@@ -5355,7 +5356,7 @@
     </row>
     <row r="138" spans="1:10">
       <c r="A138" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B138" t="s">
         <v>189</v>
@@ -5378,7 +5379,7 @@
     </row>
     <row r="139" spans="1:10">
       <c r="A139" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B139" t="s">
         <v>190</v>
@@ -5401,7 +5402,7 @@
     </row>
     <row r="140" spans="1:10">
       <c r="A140" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B140" t="s">
         <v>191</v>
@@ -5424,7 +5425,7 @@
     </row>
     <row r="141" spans="1:10">
       <c r="A141" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B141" t="s">
         <v>192</v>
@@ -5447,7 +5448,7 @@
     </row>
     <row r="142" spans="1:10">
       <c r="A142" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B142" t="s">
         <v>193</v>
@@ -5470,7 +5471,7 @@
     </row>
     <row r="143" spans="1:10">
       <c r="A143" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B143" t="s">
         <v>194</v>
@@ -5493,7 +5494,7 @@
     </row>
     <row r="144" spans="1:10">
       <c r="A144" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B144" t="s">
         <v>195</v>
@@ -5516,7 +5517,7 @@
     </row>
     <row r="145" spans="1:10">
       <c r="A145" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B145" t="s">
         <v>196</v>
@@ -5539,7 +5540,7 @@
     </row>
     <row r="146" spans="1:10">
       <c r="A146" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B146" t="s">
         <v>197</v>
@@ -5562,7 +5563,7 @@
     </row>
     <row r="147" spans="1:10">
       <c r="A147" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B147" t="s">
         <v>198</v>
@@ -5591,7 +5592,7 @@
     </row>
     <row r="148" spans="1:10">
       <c r="A148" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B148" t="s">
         <v>110</v>
@@ -5614,7 +5615,7 @@
     </row>
     <row r="149" spans="1:10">
       <c r="A149" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B149" t="s">
         <v>201</v>
@@ -5646,7 +5647,7 @@
     </row>
     <row r="150" spans="1:10">
       <c r="A150" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B150" t="s">
         <v>203</v>
@@ -5669,7 +5670,7 @@
     </row>
     <row r="151" spans="1:10">
       <c r="A151" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B151" t="s">
         <v>204</v>
@@ -5692,7 +5693,7 @@
     </row>
     <row r="152" spans="1:10">
       <c r="A152" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B152" t="s">
         <v>205</v>
@@ -5715,7 +5716,7 @@
     </row>
     <row r="153" spans="1:10">
       <c r="A153" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B153" t="s">
         <v>206</v>
@@ -5738,7 +5739,7 @@
     </row>
     <row r="154" spans="1:10">
       <c r="A154" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B154" t="s">
         <v>207</v>
@@ -5761,7 +5762,7 @@
     </row>
     <row r="155" spans="1:10">
       <c r="A155" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B155" t="s">
         <v>22</v>
@@ -5784,7 +5785,7 @@
     </row>
     <row r="156" spans="1:10">
       <c r="A156" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B156" t="s">
         <v>23</v>
@@ -5807,7 +5808,7 @@
     </row>
     <row r="157" spans="1:10">
       <c r="A157" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B157" t="s">
         <v>27</v>
@@ -5830,7 +5831,7 @@
     </row>
     <row r="158" spans="1:10">
       <c r="A158" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B158" t="s">
         <v>28</v>
@@ -5853,7 +5854,7 @@
     </row>
     <row r="159" spans="1:10">
       <c r="A159" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B159" t="s">
         <v>29</v>
@@ -5876,7 +5877,7 @@
     </row>
     <row r="160" spans="1:10">
       <c r="A160" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B160" t="s">
         <v>30</v>
@@ -5899,7 +5900,7 @@
     </row>
     <row r="161" spans="1:10">
       <c r="A161" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B161" t="s">
         <v>31</v>
@@ -5922,7 +5923,7 @@
     </row>
     <row r="162" spans="1:10">
       <c r="A162" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B162" t="s">
         <v>32</v>
@@ -5945,7 +5946,7 @@
     </row>
     <row r="163" spans="1:10">
       <c r="A163" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B163" t="s">
         <v>33</v>
@@ -5968,7 +5969,7 @@
     </row>
     <row r="164" spans="1:10">
       <c r="A164" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B164" t="s">
         <v>34</v>
@@ -5982,7 +5983,7 @@
     </row>
     <row r="165" spans="1:10">
       <c r="A165" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B165" t="s">
         <v>35</v>
@@ -6005,7 +6006,7 @@
     </row>
     <row r="166" spans="1:10">
       <c r="A166" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B166" t="s">
         <v>36</v>
@@ -6028,7 +6029,7 @@
     </row>
     <row r="167" spans="1:10">
       <c r="A167" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B167" t="s">
         <v>37</v>
@@ -6051,7 +6052,7 @@
     </row>
     <row r="168" spans="1:10">
       <c r="A168" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B168" t="s">
         <v>38</v>
@@ -6071,7 +6072,7 @@
     </row>
     <row r="169" spans="1:10">
       <c r="A169" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B169" t="s">
         <v>39</v>
@@ -6094,7 +6095,7 @@
     </row>
     <row r="170" spans="1:10">
       <c r="A170" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B170" t="s">
         <v>208</v>
@@ -6117,7 +6118,7 @@
     </row>
     <row r="171" spans="1:10">
       <c r="A171" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B171" t="s">
         <v>40</v>
@@ -6146,7 +6147,7 @@
     </row>
     <row r="172" spans="1:10">
       <c r="A172" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B172" t="s">
         <v>42</v>
@@ -6175,7 +6176,7 @@
     </row>
     <row r="173" spans="1:10">
       <c r="A173" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B173" t="s">
         <v>44</v>
@@ -6198,7 +6199,7 @@
     </row>
     <row r="174" spans="1:10">
       <c r="A174" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B174" t="s">
         <v>209</v>
@@ -6221,7 +6222,7 @@
     </row>
     <row r="175" spans="1:10">
       <c r="A175" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B175" t="s">
         <v>45</v>
@@ -6253,7 +6254,7 @@
     </row>
     <row r="176" spans="1:10">
       <c r="A176" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B176" t="s">
         <v>47</v>
@@ -6276,7 +6277,7 @@
     </row>
     <row r="177" spans="1:10">
       <c r="A177" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B177" t="s">
         <v>48</v>
@@ -6299,7 +6300,7 @@
     </row>
     <row r="178" spans="1:10">
       <c r="A178" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B178" t="s">
         <v>49</v>
@@ -6322,7 +6323,7 @@
     </row>
     <row r="179" spans="1:10">
       <c r="A179" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B179" t="s">
         <v>210</v>
@@ -6345,7 +6346,7 @@
     </row>
     <row r="180" spans="1:10">
       <c r="A180" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B180" t="s">
         <v>50</v>
@@ -6368,7 +6369,7 @@
     </row>
     <row r="181" spans="1:10">
       <c r="A181" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B181" t="s">
         <v>84</v>
@@ -6400,7 +6401,7 @@
     </row>
     <row r="182" spans="1:10">
       <c r="A182" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B182" t="s">
         <v>212</v>
@@ -6423,7 +6424,7 @@
     </row>
     <row r="183" spans="1:10">
       <c r="A183" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B183" t="s">
         <v>213</v>
@@ -6446,7 +6447,7 @@
     </row>
     <row r="184" spans="1:10">
       <c r="A184" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B184" t="s">
         <v>214</v>
@@ -6469,7 +6470,7 @@
     </row>
     <row r="185" spans="1:10">
       <c r="A185" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B185" t="s">
         <v>214</v>
@@ -6492,7 +6493,7 @@
     </row>
     <row r="186" spans="1:10">
       <c r="A186" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B186" t="s">
         <v>216</v>
@@ -6515,7 +6516,7 @@
     </row>
     <row r="187" spans="1:10">
       <c r="A187" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B187" t="s">
         <v>217</v>
@@ -6538,7 +6539,7 @@
     </row>
     <row r="188" spans="1:10">
       <c r="A188" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B188" t="s">
         <v>218</v>
@@ -6561,7 +6562,7 @@
     </row>
     <row r="189" spans="1:10">
       <c r="A189" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B189" t="s">
         <v>219</v>
@@ -6584,7 +6585,7 @@
     </row>
     <row r="190" spans="1:10">
       <c r="A190" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B190" t="s">
         <v>220</v>
@@ -6607,7 +6608,7 @@
     </row>
     <row r="191" spans="1:10">
       <c r="A191" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B191" t="s">
         <v>221</v>
@@ -6630,7 +6631,7 @@
     </row>
     <row r="192" spans="1:10">
       <c r="A192" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B192" t="s">
         <v>222</v>
@@ -6653,7 +6654,7 @@
     </row>
     <row r="193" spans="1:10">
       <c r="A193" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B193" t="s">
         <v>223</v>
@@ -6676,7 +6677,7 @@
     </row>
     <row r="194" spans="1:10">
       <c r="A194" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B194" t="s">
         <v>224</v>
@@ -6699,7 +6700,7 @@
     </row>
     <row r="195" spans="1:10">
       <c r="A195" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B195" t="s">
         <v>225</v>
@@ -6722,7 +6723,7 @@
     </row>
     <row r="196" spans="1:10">
       <c r="A196" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B196" t="s">
         <v>226</v>
@@ -6745,7 +6746,7 @@
     </row>
     <row r="197" spans="1:10">
       <c r="A197" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B197" t="s">
         <v>227</v>
@@ -6768,7 +6769,7 @@
     </row>
     <row r="198" spans="1:10">
       <c r="A198" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B198" t="s">
         <v>126</v>
@@ -6788,7 +6789,7 @@
     </row>
     <row r="199" spans="1:10">
       <c r="A199" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B199" t="s">
         <v>228</v>
@@ -6811,7 +6812,7 @@
     </row>
     <row r="200" spans="1:10">
       <c r="A200" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B200" t="s">
         <v>229</v>
@@ -6834,7 +6835,7 @@
     </row>
     <row r="201" spans="1:10">
       <c r="A201" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B201" t="s">
         <v>230</v>
@@ -6857,7 +6858,7 @@
     </row>
     <row r="202" spans="1:10">
       <c r="A202" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B202" t="s">
         <v>231</v>
@@ -6880,7 +6881,7 @@
     </row>
     <row r="203" spans="1:10">
       <c r="A203" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B203" t="s">
         <v>232</v>
@@ -6903,7 +6904,7 @@
     </row>
     <row r="204" spans="1:10">
       <c r="A204" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B204" t="s">
         <v>233</v>
@@ -6926,7 +6927,7 @@
     </row>
     <row r="205" spans="1:10">
       <c r="A205" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B205" t="s">
         <v>234</v>
@@ -6949,7 +6950,7 @@
     </row>
     <row r="206" spans="1:10">
       <c r="A206" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B206" t="s">
         <v>235</v>
@@ -6969,7 +6970,7 @@
     </row>
     <row r="207" spans="1:10">
       <c r="A207" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B207" t="s">
         <v>236</v>
@@ -6992,7 +6993,7 @@
     </row>
     <row r="208" spans="1:10">
       <c r="A208" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B208" t="s">
         <v>237</v>
@@ -7024,7 +7025,7 @@
     </row>
     <row r="209" spans="1:10">
       <c r="A209" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B209" t="s">
         <v>239</v>
@@ -7047,7 +7048,7 @@
     </row>
     <row r="210" spans="1:10">
       <c r="A210" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B210" t="s">
         <v>240</v>
@@ -7070,7 +7071,7 @@
     </row>
     <row r="211" spans="1:10">
       <c r="A211" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B211" t="s">
         <v>59</v>
@@ -7099,7 +7100,7 @@
     </row>
     <row r="212" spans="1:10">
       <c r="A212" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B212" t="s">
         <v>133</v>
@@ -7122,7 +7123,7 @@
     </row>
     <row r="213" spans="1:10">
       <c r="A213" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B213" t="s">
         <v>244</v>
@@ -7154,7 +7155,7 @@
     </row>
     <row r="214" spans="1:10">
       <c r="A214" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B214" t="s">
         <v>33</v>
@@ -7183,7 +7184,7 @@
     </row>
     <row r="215" spans="1:10">
       <c r="A215" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B215" t="s">
         <v>247</v>
@@ -7215,7 +7216,7 @@
     </row>
     <row r="216" spans="1:10">
       <c r="A216" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B216" t="s">
         <v>249</v>
@@ -7247,7 +7248,7 @@
     </row>
     <row r="217" spans="1:10">
       <c r="A217" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B217" t="s">
         <v>229</v>
@@ -7267,7 +7268,7 @@
     </row>
     <row r="218" spans="1:10">
       <c r="A218" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B218" t="s">
         <v>7</v>
@@ -7287,7 +7288,7 @@
     </row>
     <row r="219" spans="1:10">
       <c r="A219" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B219" t="s">
         <v>6</v>
@@ -7319,7 +7320,7 @@
     </row>
     <row r="220" spans="1:10">
       <c r="A220" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B220" t="s">
         <v>252</v>
@@ -7351,7 +7352,7 @@
     </row>
     <row r="221" spans="1:10">
       <c r="A221" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B221" t="s">
         <v>254</v>
@@ -7383,7 +7384,7 @@
     </row>
     <row r="222" spans="1:10">
       <c r="A222" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B222" t="s">
         <v>84</v>
@@ -7415,7 +7416,7 @@
     </row>
     <row r="223" spans="1:10">
       <c r="A223" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B223" t="s">
         <v>258</v>
@@ -7438,7 +7439,7 @@
     </row>
     <row r="224" spans="1:10">
       <c r="A224" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B224" t="s">
         <v>259</v>
@@ -7461,7 +7462,7 @@
     </row>
     <row r="225" spans="1:10">
       <c r="A225" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B225" t="s">
         <v>260</v>
@@ -7484,7 +7485,7 @@
     </row>
     <row r="226" spans="1:10">
       <c r="A226" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B226" t="s">
         <v>261</v>
@@ -7507,7 +7508,7 @@
     </row>
     <row r="227" spans="1:10">
       <c r="A227" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B227" t="s">
         <v>262</v>
@@ -7536,7 +7537,7 @@
     </row>
     <row r="228" spans="1:10">
       <c r="A228" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B228" t="s">
         <v>264</v>

</xml_diff>